<commit_message>
Working on bar chart
</commit_message>
<xml_diff>
--- a/election_poll_2016/election_poll_anon.xlsx
+++ b/election_poll_2016/election_poll_anon.xlsx
@@ -3765,7 +3765,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3773,10 +3773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U923"/>
+  <dimension ref="A1:U924"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A903" workbookViewId="0">
-      <selection activeCell="G920" sqref="G920"/>
+      <selection activeCell="G921" sqref="G921"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60416,10 +60416,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="923" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="G923">
-        <f>COUNTIF(G1:G922,"Gary Johnson")</f>
-        <v>34</v>
+    <row r="924" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="G924">
+        <f>COUNTIFS(G2:G923,"Hillary Clinton",D2:D923,"female")</f>
+        <v>400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>